<commit_message>
Committing data of 21 Aug
</commit_message>
<xml_diff>
--- a/AktivLearnAutomation/bin/dataRepository/TestData.xlsx
+++ b/AktivLearnAutomation/bin/dataRepository/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test scenarios" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS2</t>
   </si>
   <si>
     <t xml:space="preserve">Course_id</t>
@@ -294,6 +297,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -314,6 +318,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -408,19 +413,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,6 +485,11 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -499,24 +509,24 @@
   </sheetPr>
   <dimension ref="A14:C16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -524,10 +534,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,10 +545,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -565,35 +575,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -619,68 +629,71 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>20</v>
@@ -710,88 +723,90 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>30</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>42950.3958333333</v>
@@ -803,7 +818,7 @@
         <v>42961.0208333333</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>1</v>
@@ -811,10 +826,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -841,38 +856,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.8622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="27.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -899,40 +912,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.015306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="60.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -940,19 +951,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>